<commit_message>
feat: init script to download file from googledrive
</commit_message>
<xml_diff>
--- a/files/google_drive/clinical-site-registration.xlsx
+++ b/files/google_drive/clinical-site-registration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcruvolo/Github/projects-rd-recon41md/files/google_drive/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88150238-A099-2A48-B9EC-F7F4EE8B7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BC1378-A41E-EF4D-A01D-D98FD07EA1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,6 +48,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>this column is used to define the text that describes a form input. E.g., "Enter patient ID"
@@ -62,6 +63,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This column is used to provide additional context for form inputs. For example: for the "Date of registration" field, we may want to provide instructions on how to format the date - "Format date as yyyy-mm-dd"
@@ -76,6 +78,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Space to add formulas to hide or show a column based on the values in one or more columns
@@ -90,6 +93,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This column can be used to set a default value for a column or you can enter a formula
@@ -104,6 +108,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This column is used to define the way a value is calculated. These are javascript formulas
@@ -118,6 +123,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>This column is used to define formulas that validate user input.
@@ -132,6 +138,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>// To Do: add expression to retrieve current site
@@ -146,6 +153,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Change to cohort
@@ -160,6 +168,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>David - new table?
@@ -197,6 +206,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Make automatic for age 16?
@@ -211,6 +221,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Every subject should have urine and plasma. Can we set a warning or reminder that these are necessary.
@@ -225,6 +236,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Select visits from Participant data table. If other...
@@ -239,6 +251,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>changed to sample tube as for some samples (e.g. plasma) it is not the collection tube that finally needs to be registered but the sample tube with the supernatant (plasma)
@@ -253,6 +266,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>?
@@ -284,6 +298,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>What is the range of temperatures allowed? Should this field be a string rather than an integer?
@@ -298,6 +313,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>I think not so much the reason but rather specifications of the deviations
@@ -312,6 +328,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Need to add sample type and aliquot number.
@@ -326,6 +343,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>For plasma and urine select aliquot number
@@ -340,6 +358,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>If this column is dependent on the "has agreed to transfer...." column, then it would fit better in the "Patient registration" table. Unfortunately, the formulas are limited to within a table.
@@ -354,6 +373,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Should this be an ontology? We have a dataset for this: https://github.com/molgenis/molgenis-emx2/blob/master/data/_ontologies/SequencingEnrichmentKits.csv
@@ -1572,7 +1592,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1583,12 +1603,14 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1596,28 +1618,33 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1625,18 +1652,21 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <strike/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1644,6 +1674,7 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
@@ -1651,23 +1682,27 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1683,12 +1718,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1975,7 +2004,7 @@
   <dimension ref="A1:AF113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="B15" sqref="B15"/>

</xml_diff>